<commit_message>
Add output data table to monitor final result in UIPath.
</commit_message>
<xml_diff>
--- a/CardPayments.xlsx
+++ b/CardPayments.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="30540" yWindow="3990" windowWidth="14400" windowHeight="7365"/>
+    <workbookView minimized="1" xWindow="30540" yWindow="3990" windowWidth="14400" windowHeight="7365"/>
   </bookViews>
   <sheets>
     <sheet name="Pivot1" sheetId="3" r:id="rId1"/>
@@ -13,7 +13,7 @@
   </sheets>
   <calcPr calcId="162913"/>
   <pivotCaches>
-    <pivotCache cacheId="58" r:id="rId4"/>
+    <pivotCache cacheId="77" r:id="rId4"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -192,7 +192,7 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1" refreshedBy="Author" refreshedDate="45154.500825925927" createdVersion="1" refreshedVersion="6" recordCount="35">
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1" refreshedBy="Author" refreshedDate="45154.626235532407" createdVersion="1" refreshedVersion="6" recordCount="35">
   <cacheSource type="worksheet">
     <worksheetSource ref="A1:C36" sheet="Combined"/>
   </cacheSource>
@@ -408,7 +408,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="Final_Pivot" cacheId="58" dataOnRows="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Data" updatedVersion="6" asteriskTotals="1" showMultipleLabel="0" showMemberPropertyTips="0" useAutoFormatting="1" itemPrintTitles="1" showDropZones="0" indent="0" outline="1" outlineData="1">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="Final_Pivot" cacheId="77" dataOnRows="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Data" updatedVersion="6" asteriskTotals="1" showMultipleLabel="0" showMemberPropertyTips="0" useAutoFormatting="1" itemPrintTitles="1" showDropZones="0" indent="0" outline="1" outlineData="1">
   <location ref="A1:B13" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="3">
     <pivotField axis="axisRow" showAll="0" includeNewItemsInFilter="1">

</xml_diff>

<commit_message>
Add final result of project to output panel when the code is excecuted.
</commit_message>
<xml_diff>
--- a/CardPayments.xlsx
+++ b/CardPayments.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="30540" yWindow="3990" windowWidth="14400" windowHeight="7365"/>
+    <workbookView xWindow="30540" yWindow="3990" windowWidth="14400" windowHeight="7365"/>
   </bookViews>
   <sheets>
     <sheet name="Pivot1" sheetId="3" r:id="rId1"/>
@@ -13,7 +13,7 @@
   </sheets>
   <calcPr calcId="162913"/>
   <pivotCaches>
-    <pivotCache cacheId="77" r:id="rId4"/>
+    <pivotCache cacheId="89" r:id="rId4"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="28">
   <si>
     <t>Expense</t>
   </si>
@@ -116,6 +116,9 @@
   </si>
   <si>
     <t>Sum of Value</t>
+  </si>
+  <si>
+    <t>Expense %</t>
   </si>
 </sst>
 </file>
@@ -126,7 +129,7 @@
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -137,6 +140,13 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -163,7 +173,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
@@ -173,6 +183,7 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="10" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -192,7 +203,7 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1" refreshedBy="Author" refreshedDate="45154.626235532407" createdVersion="1" refreshedVersion="6" recordCount="35">
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1" refreshedBy="Author" refreshedDate="45154.643607175924" createdVersion="1" refreshedVersion="6" recordCount="35">
   <cacheSource type="worksheet">
     <worksheetSource ref="A1:C36" sheet="Combined"/>
   </cacheSource>
@@ -408,7 +419,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="Final_Pivot" cacheId="77" dataOnRows="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Data" updatedVersion="6" asteriskTotals="1" showMultipleLabel="0" showMemberPropertyTips="0" useAutoFormatting="1" itemPrintTitles="1" showDropZones="0" indent="0" outline="1" outlineData="1">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="Final_Pivot" cacheId="89" dataOnRows="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Data" updatedVersion="6" asteriskTotals="1" showMultipleLabel="0" showMemberPropertyTips="0" useAutoFormatting="1" itemPrintTitles="1" showDropZones="0" indent="0" outline="1" outlineData="1">
   <location ref="A1:B13" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="3">
     <pivotField axis="axisRow" showAll="0" includeNewItemsInFilter="1">
@@ -785,6 +796,9 @@
       <c r="B1" t="s">
         <v>26</v>
       </c>
+      <c r="C1" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
@@ -793,9 +807,8 @@
       <c r="B2" s="6">
         <v>354</v>
       </c>
-      <c r="C2">
-        <f t="shared" ref="C2:C12" si="0">(B2/$B$13)*100</f>
-        <v>1.7070936008101463</v>
+      <c r="C2" s="7">
+        <v>1.7070936008101462E-2</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -805,9 +818,8 @@
       <c r="B3" s="6">
         <v>1283</v>
       </c>
-      <c r="C3">
-        <f t="shared" si="0"/>
-        <v>6.1870087283599364</v>
+      <c r="C3" s="7">
+        <v>6.1870087283599363E-2</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
@@ -817,9 +829,8 @@
       <c r="B4" s="6">
         <v>551</v>
       </c>
-      <c r="C4">
-        <f t="shared" si="0"/>
-        <v>2.6570863673626848</v>
+      <c r="C4" s="7">
+        <v>2.6570863673626849E-2</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
@@ -829,9 +840,8 @@
       <c r="B5" s="6">
         <v>5178</v>
       </c>
-      <c r="C5">
-        <f t="shared" si="0"/>
-        <v>24.969860635578918</v>
+      <c r="C5" s="7">
+        <v>0.24969860635578917</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
@@ -841,9 +851,8 @@
       <c r="B6" s="6">
         <v>452</v>
       </c>
-      <c r="C6">
-        <f t="shared" si="0"/>
-        <v>2.1796788349327292</v>
+      <c r="C6" s="7">
+        <v>2.179678834932729E-2</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
@@ -853,9 +862,8 @@
       <c r="B7" s="6">
         <v>425</v>
       </c>
-      <c r="C7">
-        <f t="shared" si="0"/>
-        <v>2.04947678063365</v>
+      <c r="C7" s="7">
+        <v>2.0494767806336502E-2</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
@@ -865,9 +873,8 @@
       <c r="B8" s="6">
         <v>100</v>
       </c>
-      <c r="C8">
-        <f t="shared" si="0"/>
-        <v>0.48222983073732945</v>
+      <c r="C8" s="7">
+        <v>4.8222983073732944E-3</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
@@ -877,9 +884,8 @@
       <c r="B9" s="6">
         <v>394</v>
       </c>
-      <c r="C9">
-        <f t="shared" si="0"/>
-        <v>1.8999855331050779</v>
+      <c r="C9" s="7">
+        <v>1.899985533105078E-2</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
@@ -889,9 +895,8 @@
       <c r="B10" s="6">
         <v>7500</v>
       </c>
-      <c r="C10">
-        <f t="shared" si="0"/>
-        <v>36.167237305299707</v>
+      <c r="C10" s="7">
+        <v>0.36167237305299704</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
@@ -901,9 +906,8 @@
       <c r="B11" s="6">
         <v>2500</v>
       </c>
-      <c r="C11">
-        <f t="shared" si="0"/>
-        <v>12.055745768433235</v>
+      <c r="C11" s="7">
+        <v>0.12055745768433235</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
@@ -913,9 +917,8 @@
       <c r="B12" s="6">
         <v>2000</v>
       </c>
-      <c r="C12">
-        <f t="shared" si="0"/>
-        <v>9.6445966147465878</v>
+      <c r="C12" s="7">
+        <v>9.6445966147465881E-2</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
@@ -928,6 +931,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Add new Sequence Challenge-1_Part-3
</commit_message>
<xml_diff>
--- a/CardPayments.xlsx
+++ b/CardPayments.xlsx
@@ -13,7 +13,7 @@
   </sheets>
   <calcPr calcId="162913"/>
   <pivotCaches>
-    <pivotCache cacheId="89" r:id="rId4"/>
+    <pivotCache cacheId="6" r:id="rId4"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -203,7 +203,7 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1" refreshedBy="Author" refreshedDate="45154.643607175924" createdVersion="1" refreshedVersion="6" recordCount="35">
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1" refreshedBy="Author" refreshedDate="45156.383638541665" createdVersion="1" refreshedVersion="6" recordCount="35">
   <cacheSource type="worksheet">
     <worksheetSource ref="A1:C36" sheet="Combined"/>
   </cacheSource>
@@ -419,7 +419,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="Final_Pivot" cacheId="89" dataOnRows="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Data" updatedVersion="6" asteriskTotals="1" showMultipleLabel="0" showMemberPropertyTips="0" useAutoFormatting="1" itemPrintTitles="1" showDropZones="0" indent="0" outline="1" outlineData="1">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="Final_Pivot" cacheId="6" dataOnRows="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Data" updatedVersion="6" asteriskTotals="1" showMultipleLabel="0" showMemberPropertyTips="0" useAutoFormatting="1" itemPrintTitles="1" showDropZones="0" indent="0" outline="1" outlineData="1">
   <location ref="A1:B13" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="3">
     <pivotField axis="axisRow" showAll="0" includeNewItemsInFilter="1">

</xml_diff>

<commit_message>
Add the sum of total percentages in expenses column
</commit_message>
<xml_diff>
--- a/CardPayments.xlsx
+++ b/CardPayments.xlsx
@@ -173,7 +173,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
@@ -184,6 +184,7 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="10" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -203,7 +204,7 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1" refreshedBy="Author" refreshedDate="45156.383638541665" createdVersion="1" refreshedVersion="6" recordCount="35">
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1" refreshedBy="Author" refreshedDate="45156.453220138887" createdVersion="1" refreshedVersion="6" recordCount="35">
   <cacheSource type="worksheet">
     <worksheetSource ref="A1:C36" sheet="Combined"/>
   </cacheSource>
@@ -780,7 +781,7 @@
   <dimension ref="A1:C13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:B13"/>
+      <selection activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -927,6 +928,10 @@
       </c>
       <c r="B13" s="6">
         <v>20737</v>
+      </c>
+      <c r="C13" s="8">
+        <f>SUM(C2:C12)</f>
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>